<commit_message>
added functionlity to see pedidos details in depth
</commit_message>
<xml_diff>
--- a/Utilidades/ListaProductosExtras.xlsx
+++ b/Utilidades/ListaProductosExtras.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paddy\Desktop\Facil Digital\CambaCuaVet\Utilidades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paddy\Desktop\Facil Digital\CambaCuaVet\CambaCua-Admin-Dash\Utilidades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0820A48E-1119-4843-89EE-442C24582E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77662F6E-F44B-42C6-99F8-E4857F2D9898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18540" yWindow="0" windowWidth="10365" windowHeight="15585" xr2:uid="{419744A9-FE47-4088-9E9E-09345077851C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{419744A9-FE47-4088-9E9E-09345077851C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F9FDF9-DC33-4E41-864D-B4E14EFB9112}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>